<commit_message>
Update stock count cells
</commit_message>
<xml_diff>
--- a/templates/stock_count.xlsx
+++ b/templates/stock_count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romuald/Documents/Work/medic/app-services-team/stock-monitoring/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACD1363-EC2D-D748-BA64-FDE2D56F2E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0685671-7020-8C48-9310-EAA22D1594B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29340" windowHeight="17700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>type</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>NO_LABEL</t>
-  </si>
-  <si>
-    <t>db:health_center</t>
   </si>
   <si>
     <t>_id</t>
@@ -307,12 +304,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -644,19 +640,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="61.83203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="5"/>
-    <col min="5" max="5" width="21.83203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="5"/>
-    <col min="9" max="9" width="19.5" style="5" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="23.83203125" style="5" customWidth="1"/>
-    <col min="12" max="13" width="11.5" style="5"/>
-    <col min="14" max="16384" width="11.5" style="4"/>
+    <col min="1" max="1" width="30.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="61.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="4"/>
+    <col min="5" max="5" width="21.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="4"/>
+    <col min="9" max="9" width="19.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="11.5" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.2">
@@ -696,366 +691,301 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="F6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10" t="s">
+      <c r="B21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11" t="s">
+      <c r="B22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="5" t="s">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
+      <c r="A24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -1094,39 +1024,39 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>61</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update template and ensure it converts
</commit_message>
<xml_diff>
--- a/templates/stock_count.xlsx
+++ b/templates/stock_count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romuald/Documents/Work/medic/app-services-team/stock-monitoring/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0685671-7020-8C48-9310-EAA22D1594B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FAD504-E7A3-1842-B980-A7E58E4BBF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29340" windowHeight="17700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>type</t>
   </si>
@@ -116,9 +116,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>db-object</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -132,12 +129,6 @@
   </si>
   <si>
     <t>../inputs/contact/_id</t>
-  </si>
-  <si>
-    <t>is_mch_instance</t>
-  </si>
-  <si>
-    <t>instance('contact-summary')/context/isMCHInstance</t>
   </si>
   <si>
     <t>items</t>
@@ -219,7 +210,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -242,13 +233,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -310,7 +294,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -318,6 +301,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -691,34 +675,34 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -752,42 +736,38 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -798,52 +778,52 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="A8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>26</v>
@@ -852,138 +832,124 @@
         <v>21</v>
       </c>
       <c r="I12" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="C15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8" t="s">
         <v>36</v>
       </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B20" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
+      <c r="A23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1024,39 +990,39 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>